<commit_message>
add report for Lab02
</commit_message>
<xml_diff>
--- a/6_Reports/Risc-V指令整理.xlsx
+++ b/6_Reports/Risc-V指令整理.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerrygu/Desktop/Study/大三下/体系结构 /Lab Info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerrygu/Desktop/Study/大三下/体系结构 /Lab Info/6_Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714A4DBA-3146-7A49-B737-3CBA5A8E73E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E30B66-F5FD-E241-80CC-DC245494541E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19040" xr2:uid="{FB31A1F9-B16A-4445-9924-0591DA43B4E1}"/>
   </bookViews>
@@ -629,8 +629,8 @@
   </sheetPr>
   <dimension ref="A1:AU78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2911,7 +2911,7 @@
         <v>43</v>
       </c>
       <c r="K35" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L35" s="8">
         <v>0</v>
@@ -2956,7 +2956,7 @@
         <v>44</v>
       </c>
       <c r="K36" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L36" s="8">
         <v>0</v>
@@ -3001,7 +3001,7 @@
         <v>45</v>
       </c>
       <c r="K37" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L37" s="8">
         <v>0</v>
@@ -3046,7 +3046,7 @@
         <v>46</v>
       </c>
       <c r="K38" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L38" s="8">
         <v>0</v>
@@ -3091,7 +3091,7 @@
         <v>47</v>
       </c>
       <c r="K39" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L39" s="8">
         <v>0</v>
@@ -3136,7 +3136,7 @@
         <v>48</v>
       </c>
       <c r="K40" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L40" s="8">
         <v>0</v>

</xml_diff>